<commit_message>
:construction: write about ulmanssubgraph Algorithm
</commit_message>
<xml_diff>
--- a/Kapitel/Kapitel-GraphLib/Dateien/Subisomophism.xlsx
+++ b/Kapitel/Kapitel-GraphLib/Dateien/Subisomophism.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christoph Weberbauer\Documents\Chrisi\Programmieren\matura-arbeit\Kapitel\Kapitel-GraphLib\Dateien\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9949AFB-73BB-40A7-8542-16C64ED855C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A9A860-03A3-45E1-8C70-89D1058EAFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="4170" windowWidth="21600" windowHeight="11505" xr2:uid="{6F570890-30DC-4F09-BED8-0D7C34AA1E89}"/>
+    <workbookView xWindow="4515" yWindow="4245" windowWidth="21600" windowHeight="11505" xr2:uid="{6F570890-30DC-4F09-BED8-0D7C34AA1E89}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="2">
   <si>
     <t>N-Graph</t>
   </si>
@@ -134,14 +134,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -457,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{370F70E0-C2FA-4672-B496-410DDF30F3C8}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="235" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="235" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,21 +473,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+      <c r="A2" s="5"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3">
         <v>1</v>
@@ -509,7 +509,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="5"/>
       <c r="B3" s="3">
         <v>1</v>
       </c>
@@ -533,7 +533,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="3">
         <v>2</v>
       </c>
@@ -557,7 +557,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="3">
         <v>3</v>
       </c>
@@ -581,7 +581,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="3">
         <v>4</v>
       </c>
@@ -605,21 +605,21 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="A10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="5"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3">
         <v>1</v>
@@ -641,7 +641,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="A12" s="5"/>
       <c r="B12" s="3">
         <v>1</v>
       </c>
@@ -665,7 +665,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+      <c r="A13" s="5"/>
       <c r="B13" s="3">
         <v>2</v>
       </c>
@@ -689,7 +689,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
+      <c r="A14" s="5"/>
       <c r="B14" s="3">
         <v>3</v>
       </c>
@@ -713,7 +713,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+      <c r="A15" s="5"/>
       <c r="B15" s="3">
         <v>4</v>
       </c>
@@ -737,21 +737,21 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
+      <c r="A18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+      <c r="A19" s="5"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3">
         <v>1</v>
@@ -773,7 +773,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+      <c r="A20" s="5"/>
       <c r="B20" s="3">
         <v>1</v>
       </c>
@@ -797,7 +797,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+      <c r="A21" s="5"/>
       <c r="B21" s="3">
         <v>2</v>
       </c>
@@ -821,7 +821,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
+      <c r="A22" s="5"/>
       <c r="B22" s="3">
         <v>3</v>
       </c>
@@ -845,7 +845,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
+      <c r="A23" s="5"/>
       <c r="B23" s="3">
         <v>4</v>
       </c>
@@ -868,8 +868,142 @@
         <v>0</v>
       </c>
     </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3">
+        <v>2</v>
+      </c>
+      <c r="E27" s="3">
+        <v>3</v>
+      </c>
+      <c r="F27" s="3">
+        <v>4</v>
+      </c>
+      <c r="G27" s="3">
+        <v>5</v>
+      </c>
+      <c r="H27" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="3">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="3">
+        <v>2</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="3">
+        <v>3</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="3">
+        <v>4</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="B26:H26"/>
     <mergeCell ref="B18:H18"/>
     <mergeCell ref="B10:H10"/>
     <mergeCell ref="B1:H1"/>

</xml_diff>